<commit_message>
Created Comparison Table (Blank)
</commit_message>
<xml_diff>
--- a/Assignment3/Comparison of Algorithms.xlsx
+++ b/Assignment3/Comparison of Algorithms.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shrawan/Desktop/Vaibhavi/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vrangar3\Documents\GitHub\CSE-415\Assignment3\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9960" yWindow="2840" windowWidth="18840" windowHeight="13640" tabRatio="500"/>
+    <workbookView xWindow="9960" yWindow="2844" windowWidth="18840" windowHeight="13644" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,38 +27,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
-  <si>
-    <t>terminal input</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="25">
   <si>
     <t>problem</t>
   </si>
   <si>
-    <t>algorithm</t>
-  </si>
-  <si>
     <t>initial_state</t>
   </si>
   <si>
-    <t>optimal_path_length</t>
-  </si>
-  <si>
-    <t>num_expanded_nodes</t>
-  </si>
-  <si>
     <t>heuristic</t>
   </si>
   <si>
-    <t xml:space="preserve">python AStar.py </t>
-  </si>
-  <si>
     <t>EightPuzzleWithHeuristics</t>
   </si>
   <si>
-    <t>AStar</t>
-  </si>
-  <si>
     <t>h_hamming</t>
   </si>
   <si>
@@ -69,12 +51,63 @@
   </si>
   <si>
     <t>h_custom</t>
+  </si>
+  <si>
+    <t>initial_state_file</t>
+  </si>
+  <si>
+    <t>algo</t>
+  </si>
+  <si>
+    <t>puzzle0</t>
+  </si>
+  <si>
+    <t>puzzle1a</t>
+  </si>
+  <si>
+    <t>puzzle2a</t>
+  </si>
+  <si>
+    <t>puzzle4a</t>
+  </si>
+  <si>
+    <t>puzzle10a</t>
+  </si>
+  <si>
+    <t>puzzle12a</t>
+  </si>
+  <si>
+    <t>puzzle14a</t>
+  </si>
+  <si>
+    <t>puzzle16a</t>
+  </si>
+  <si>
+    <t>terminal_input</t>
+  </si>
+  <si>
+    <t>AStar.py</t>
+  </si>
+  <si>
+    <t>ItrBFS.py</t>
+  </si>
+  <si>
+    <t>BasicEightPuzzle</t>
+  </si>
+  <si>
+    <t>path_len</t>
+  </si>
+  <si>
+    <t>searched_nodes</t>
+  </si>
+  <si>
+    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -84,20 +117,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -109,14 +146,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -124,6 +163,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -392,75 +434,750 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.5" customWidth="1"/>
-    <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="26.1640625" customWidth="1"/>
-    <col min="4" max="4" width="19.33203125" customWidth="1"/>
-    <col min="5" max="5" width="25" customWidth="1"/>
-    <col min="6" max="6" width="20.83203125" customWidth="1"/>
+    <col min="1" max="1" width="23.69921875" customWidth="1"/>
+    <col min="2" max="2" width="10.69921875" customWidth="1"/>
+    <col min="3" max="3" width="13.59765625" customWidth="1"/>
+    <col min="4" max="4" width="19.3984375" customWidth="1"/>
+    <col min="5" max="5" width="9.09765625" customWidth="1"/>
+    <col min="6" max="6" width="14.5" customWidth="1"/>
+    <col min="8" max="8" width="60.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H2" t="str">
+        <f t="shared" ref="H2:H41" si="0" xml:space="preserve"> "python "&amp;B2&amp;" "&amp;A2&amp;" "&amp;G2&amp;" "&amp;C2</f>
+        <v>python AStar.py EightPuzzleWithHeuristics h_hamming puzzle0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" t="str">
+        <f t="shared" si="0"/>
+        <v>python AStar.py EightPuzzleWithHeuristics h_hamming puzzle1a</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" si="0"/>
+        <v>python AStar.py EightPuzzleWithHeuristics h_hamming puzzle2a</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" si="0"/>
+        <v>python AStar.py EightPuzzleWithHeuristics h_hamming puzzle4a</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="0"/>
+        <v>python AStar.py EightPuzzleWithHeuristics h_hamming puzzle10a</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" si="0"/>
+        <v>python AStar.py EightPuzzleWithHeuristics h_hamming puzzle12a</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="0"/>
+        <v>python AStar.py EightPuzzleWithHeuristics h_hamming puzzle14a</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" t="s">
+        <v>4</v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" si="0"/>
+        <v>python AStar.py EightPuzzleWithHeuristics h_hamming puzzle16a</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H10" t="str">
+        <f t="shared" si="0"/>
+        <v>python AStar.py EightPuzzleWithHeuristics h_euclidean puzzle0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" t="s">
+        <v>5</v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" si="0"/>
+        <v>python AStar.py EightPuzzleWithHeuristics h_euclidean puzzle1a</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" t="s">
+        <v>5</v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" si="0"/>
+        <v>python AStar.py EightPuzzleWithHeuristics h_euclidean puzzle2a</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" t="s">
+        <v>5</v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" si="0"/>
+        <v>python AStar.py EightPuzzleWithHeuristics h_euclidean puzzle4a</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14" t="s">
+        <v>5</v>
+      </c>
+      <c r="H14" t="str">
+        <f t="shared" si="0"/>
+        <v>python AStar.py EightPuzzleWithHeuristics h_euclidean puzzle10a</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G15" t="s">
+        <v>5</v>
+      </c>
+      <c r="H15" t="str">
+        <f t="shared" si="0"/>
+        <v>python AStar.py EightPuzzleWithHeuristics h_euclidean puzzle12a</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" t="s">
+        <v>5</v>
+      </c>
+      <c r="H16" t="str">
+        <f t="shared" si="0"/>
+        <v>python AStar.py EightPuzzleWithHeuristics h_euclidean puzzle14a</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" t="s">
+        <v>17</v>
+      </c>
+      <c r="G17" t="s">
+        <v>5</v>
+      </c>
+      <c r="H17" t="str">
+        <f t="shared" si="0"/>
+        <v>python AStar.py EightPuzzleWithHeuristics h_euclidean puzzle16a</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="H18" t="str">
+        <f t="shared" si="0"/>
+        <v>python AStar.py EightPuzzleWithHeuristics h_manhattan puzzle0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19" t="s">
+        <v>6</v>
+      </c>
+      <c r="H19" t="str">
+        <f t="shared" si="0"/>
+        <v>python AStar.py EightPuzzleWithHeuristics h_manhattan puzzle1a</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" t="s">
+        <v>6</v>
+      </c>
+      <c r="H20" t="str">
+        <f t="shared" si="0"/>
+        <v>python AStar.py EightPuzzleWithHeuristics h_manhattan puzzle2a</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" t="s">
+        <v>6</v>
+      </c>
+      <c r="H21" t="str">
+        <f t="shared" si="0"/>
+        <v>python AStar.py EightPuzzleWithHeuristics h_manhattan puzzle4a</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" t="s">
+        <v>6</v>
+      </c>
+      <c r="H22" t="str">
+        <f t="shared" si="0"/>
+        <v>python AStar.py EightPuzzleWithHeuristics h_manhattan puzzle10a</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" t="s">
+        <v>15</v>
+      </c>
+      <c r="G23" t="s">
+        <v>6</v>
+      </c>
+      <c r="H23" t="str">
+        <f t="shared" si="0"/>
+        <v>python AStar.py EightPuzzleWithHeuristics h_manhattan puzzle12a</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" t="s">
+        <v>16</v>
+      </c>
+      <c r="G24" t="s">
+        <v>6</v>
+      </c>
+      <c r="H24" t="str">
+        <f t="shared" si="0"/>
+        <v>python AStar.py EightPuzzleWithHeuristics h_manhattan puzzle14a</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" t="s">
+        <v>17</v>
+      </c>
+      <c r="G25" t="s">
+        <v>6</v>
+      </c>
+      <c r="H25" t="str">
+        <f t="shared" si="0"/>
+        <v>python AStar.py EightPuzzleWithHeuristics h_manhattan puzzle16a</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" t="s">
+        <v>10</v>
+      </c>
+      <c r="G26" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="H26" t="str">
+        <f t="shared" si="0"/>
+        <v>python AStar.py EightPuzzleWithHeuristics h_custom puzzle0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" t="s">
+        <v>19</v>
+      </c>
+      <c r="C27" t="s">
+        <v>11</v>
+      </c>
+      <c r="G27" t="s">
+        <v>7</v>
+      </c>
+      <c r="H27" t="str">
+        <f t="shared" si="0"/>
+        <v>python AStar.py EightPuzzleWithHeuristics h_custom puzzle1a</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>3</v>
+      </c>
+      <c r="B28" t="s">
+        <v>19</v>
+      </c>
+      <c r="C28" t="s">
+        <v>12</v>
+      </c>
+      <c r="G28" t="s">
+        <v>7</v>
+      </c>
+      <c r="H28" t="str">
+        <f t="shared" si="0"/>
+        <v>python AStar.py EightPuzzleWithHeuristics h_custom puzzle2a</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29" t="s">
+        <v>19</v>
+      </c>
+      <c r="C29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G29" t="s">
+        <v>7</v>
+      </c>
+      <c r="H29" t="str">
+        <f t="shared" si="0"/>
+        <v>python AStar.py EightPuzzleWithHeuristics h_custom puzzle4a</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>3</v>
+      </c>
+      <c r="B30" t="s">
+        <v>19</v>
+      </c>
+      <c r="C30" t="s">
+        <v>14</v>
+      </c>
+      <c r="G30" t="s">
+        <v>7</v>
+      </c>
+      <c r="H30" t="str">
+        <f t="shared" si="0"/>
+        <v>python AStar.py EightPuzzleWithHeuristics h_custom puzzle10a</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>3</v>
+      </c>
+      <c r="B31" t="s">
+        <v>19</v>
+      </c>
+      <c r="C31" t="s">
+        <v>15</v>
+      </c>
+      <c r="G31" t="s">
+        <v>7</v>
+      </c>
+      <c r="H31" t="str">
+        <f t="shared" si="0"/>
+        <v>python AStar.py EightPuzzleWithHeuristics h_custom puzzle12a</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>3</v>
+      </c>
+      <c r="B32" t="s">
+        <v>19</v>
+      </c>
+      <c r="C32" t="s">
+        <v>16</v>
+      </c>
+      <c r="G32" t="s">
+        <v>7</v>
+      </c>
+      <c r="H32" t="str">
+        <f t="shared" si="0"/>
+        <v>python AStar.py EightPuzzleWithHeuristics h_custom puzzle14a</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33" t="s">
+        <v>17</v>
+      </c>
+      <c r="G33" t="s">
+        <v>7</v>
+      </c>
+      <c r="H33" t="str">
+        <f t="shared" si="0"/>
+        <v>python AStar.py EightPuzzleWithHeuristics h_custom puzzle16a</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>21</v>
+      </c>
+      <c r="B34" t="s">
+        <v>20</v>
+      </c>
+      <c r="C34" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G3" t="s">
+      <c r="H34" t="str">
+        <f t="shared" si="0"/>
+        <v>python ItrBFS.py BasicEightPuzzle  puzzle0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>21</v>
+      </c>
+      <c r="B35" t="s">
+        <v>20</v>
+      </c>
+      <c r="C35" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G4" t="s">
+      <c r="H35" t="str">
+        <f t="shared" si="0"/>
+        <v>python ItrBFS.py BasicEightPuzzle  puzzle1a</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>21</v>
+      </c>
+      <c r="B36" t="s">
+        <v>20</v>
+      </c>
+      <c r="C36" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G5" t="s">
+      <c r="H36" t="str">
+        <f t="shared" si="0"/>
+        <v>python ItrBFS.py BasicEightPuzzle  puzzle2a</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>21</v>
+      </c>
+      <c r="B37" t="s">
+        <v>20</v>
+      </c>
+      <c r="C37" t="s">
         <v>13</v>
+      </c>
+      <c r="H37" t="str">
+        <f t="shared" si="0"/>
+        <v>python ItrBFS.py BasicEightPuzzle  puzzle4a</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>21</v>
+      </c>
+      <c r="B38" t="s">
+        <v>20</v>
+      </c>
+      <c r="C38" t="s">
+        <v>14</v>
+      </c>
+      <c r="H38" t="str">
+        <f t="shared" si="0"/>
+        <v>python ItrBFS.py BasicEightPuzzle  puzzle10a</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>21</v>
+      </c>
+      <c r="B39" t="s">
+        <v>20</v>
+      </c>
+      <c r="C39" t="s">
+        <v>15</v>
+      </c>
+      <c r="H39" t="str">
+        <f t="shared" si="0"/>
+        <v>python ItrBFS.py BasicEightPuzzle  puzzle12a</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>21</v>
+      </c>
+      <c r="B40" t="s">
+        <v>20</v>
+      </c>
+      <c r="C40" t="s">
+        <v>16</v>
+      </c>
+      <c r="H40" t="str">
+        <f t="shared" si="0"/>
+        <v>python ItrBFS.py BasicEightPuzzle  puzzle14a</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>21</v>
+      </c>
+      <c r="B41" t="s">
+        <v>20</v>
+      </c>
+      <c r="C41" t="s">
+        <v>17</v>
+      </c>
+      <c r="H41" t="str">
+        <f t="shared" si="0"/>
+        <v>python ItrBFS.py BasicEightPuzzle  puzzle16a</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Final Changes for submission, corrected Custom Heuristic
</commit_message>
<xml_diff>
--- a/Assignment3/Comparison of Algorithms.xlsx
+++ b/Assignment3/Comparison of Algorithms.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-200" yWindow="440" windowWidth="14720" windowHeight="13900" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -187,9 +187,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="98">
+  <cellStyleXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -291,7 +295,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="98">
+  <cellStyles count="102">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -340,6 +344,8 @@
     <cellStyle name="Followed Hyperlink" xfId="93" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="101" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -388,6 +394,8 @@
     <cellStyle name="Hyperlink" xfId="92" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="94" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="96" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="98" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="100" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -669,8 +677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="D21" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -733,7 +741,7 @@
         <v>4</v>
       </c>
       <c r="H2" t="str">
-        <f xml:space="preserve"> "python "&amp;B2&amp;" "&amp;A2&amp;" "&amp;G2&amp;" "&amp;C2</f>
+        <f t="shared" ref="H2:H49" si="0" xml:space="preserve"> "python "&amp;B2&amp;" "&amp;A2&amp;" "&amp;G2&amp;" "&amp;C2</f>
         <v>python AStar.py EightPuzzleWithHeuristics h_hamming puzzle0</v>
       </c>
     </row>
@@ -760,7 +768,7 @@
         <v>5</v>
       </c>
       <c r="H3" t="str">
-        <f xml:space="preserve"> "python "&amp;B3&amp;" "&amp;A3&amp;" "&amp;G3&amp;" "&amp;C3</f>
+        <f t="shared" si="0"/>
         <v>python AStar.py EightPuzzleWithHeuristics h_euclidean puzzle0</v>
       </c>
     </row>
@@ -787,7 +795,7 @@
         <v>6</v>
       </c>
       <c r="H4" t="str">
-        <f xml:space="preserve"> "python "&amp;B4&amp;" "&amp;A4&amp;" "&amp;G4&amp;" "&amp;C4</f>
+        <f t="shared" si="0"/>
         <v>python AStar.py EightPuzzleWithHeuristics h_manhattan puzzle0</v>
       </c>
     </row>
@@ -814,7 +822,7 @@
         <v>7</v>
       </c>
       <c r="H5" t="str">
-        <f xml:space="preserve"> "python "&amp;B5&amp;" "&amp;A5&amp;" "&amp;G5&amp;" "&amp;C5</f>
+        <f t="shared" si="0"/>
         <v>python AStar.py EightPuzzleWithHeuristics h_custom puzzle0</v>
       </c>
     </row>
@@ -841,7 +849,7 @@
         <v>4</v>
       </c>
       <c r="H6" t="str">
-        <f xml:space="preserve"> "python "&amp;B6&amp;" "&amp;A6&amp;" "&amp;G6&amp;" "&amp;C6</f>
+        <f t="shared" si="0"/>
         <v>python AStar.py EightPuzzleWithHeuristics h_hamming puzzle1a</v>
       </c>
     </row>
@@ -868,7 +876,7 @@
         <v>5</v>
       </c>
       <c r="H7" t="str">
-        <f xml:space="preserve"> "python "&amp;B7&amp;" "&amp;A7&amp;" "&amp;G7&amp;" "&amp;C7</f>
+        <f t="shared" si="0"/>
         <v>python AStar.py EightPuzzleWithHeuristics h_euclidean puzzle1a</v>
       </c>
     </row>
@@ -895,7 +903,7 @@
         <v>6</v>
       </c>
       <c r="H8" t="str">
-        <f xml:space="preserve"> "python "&amp;B8&amp;" "&amp;A8&amp;" "&amp;G8&amp;" "&amp;C8</f>
+        <f t="shared" si="0"/>
         <v>python AStar.py EightPuzzleWithHeuristics h_manhattan puzzle1a</v>
       </c>
     </row>
@@ -922,7 +930,7 @@
         <v>7</v>
       </c>
       <c r="H9" t="str">
-        <f xml:space="preserve"> "python "&amp;B9&amp;" "&amp;A9&amp;" "&amp;G9&amp;" "&amp;C9</f>
+        <f t="shared" si="0"/>
         <v>python AStar.py EightPuzzleWithHeuristics h_custom puzzle1a</v>
       </c>
     </row>
@@ -946,7 +954,7 @@
         <v>2</v>
       </c>
       <c r="H10" t="str">
-        <f xml:space="preserve"> "python "&amp;B10&amp;" "&amp;A10&amp;" "&amp;G10&amp;" "&amp;C10</f>
+        <f t="shared" si="0"/>
         <v>python ItrBFS.py EightPuzzleWithHeuristics  puzzle0</v>
       </c>
     </row>
@@ -973,7 +981,7 @@
         <v>4</v>
       </c>
       <c r="H11" t="str">
-        <f xml:space="preserve"> "python "&amp;B11&amp;" "&amp;A11&amp;" "&amp;G11&amp;" "&amp;C11</f>
+        <f t="shared" si="0"/>
         <v>python AStar.py EightPuzzleWithHeuristics h_hamming puzzle2a</v>
       </c>
     </row>
@@ -1000,7 +1008,7 @@
         <v>5</v>
       </c>
       <c r="H12" t="str">
-        <f xml:space="preserve"> "python "&amp;B12&amp;" "&amp;A12&amp;" "&amp;G12&amp;" "&amp;C12</f>
+        <f t="shared" si="0"/>
         <v>python AStar.py EightPuzzleWithHeuristics h_euclidean puzzle2a</v>
       </c>
     </row>
@@ -1027,7 +1035,7 @@
         <v>6</v>
       </c>
       <c r="H13" t="str">
-        <f xml:space="preserve"> "python "&amp;B13&amp;" "&amp;A13&amp;" "&amp;G13&amp;" "&amp;C13</f>
+        <f t="shared" si="0"/>
         <v>python AStar.py EightPuzzleWithHeuristics h_manhattan puzzle2a</v>
       </c>
     </row>
@@ -1054,7 +1062,7 @@
         <v>7</v>
       </c>
       <c r="H14" t="str">
-        <f xml:space="preserve"> "python "&amp;B14&amp;" "&amp;A14&amp;" "&amp;G14&amp;" "&amp;C14</f>
+        <f t="shared" si="0"/>
         <v>python AStar.py EightPuzzleWithHeuristics h_custom puzzle2a</v>
       </c>
     </row>
@@ -1081,7 +1089,7 @@
         <v>4</v>
       </c>
       <c r="H15" t="str">
-        <f xml:space="preserve"> "python "&amp;B15&amp;" "&amp;A15&amp;" "&amp;G15&amp;" "&amp;C15</f>
+        <f t="shared" si="0"/>
         <v>python AStar.py EightPuzzleWithHeuristics h_hamming puzzle4a</v>
       </c>
     </row>
@@ -1108,7 +1116,7 @@
         <v>5</v>
       </c>
       <c r="H16" t="str">
-        <f xml:space="preserve"> "python "&amp;B16&amp;" "&amp;A16&amp;" "&amp;G16&amp;" "&amp;C16</f>
+        <f t="shared" si="0"/>
         <v>python AStar.py EightPuzzleWithHeuristics h_euclidean puzzle4a</v>
       </c>
     </row>
@@ -1135,7 +1143,7 @@
         <v>6</v>
       </c>
       <c r="H17" t="str">
-        <f xml:space="preserve"> "python "&amp;B17&amp;" "&amp;A17&amp;" "&amp;G17&amp;" "&amp;C17</f>
+        <f t="shared" si="0"/>
         <v>python AStar.py EightPuzzleWithHeuristics h_manhattan puzzle4a</v>
       </c>
     </row>
@@ -1162,7 +1170,7 @@
         <v>7</v>
       </c>
       <c r="H18" t="str">
-        <f xml:space="preserve"> "python "&amp;B18&amp;" "&amp;A18&amp;" "&amp;G18&amp;" "&amp;C18</f>
+        <f t="shared" si="0"/>
         <v>python AStar.py EightPuzzleWithHeuristics h_custom puzzle4a</v>
       </c>
     </row>
@@ -1189,7 +1197,7 @@
         <v>4</v>
       </c>
       <c r="H19" t="str">
-        <f xml:space="preserve"> "python "&amp;B19&amp;" "&amp;A19&amp;" "&amp;G19&amp;" "&amp;C19</f>
+        <f t="shared" si="0"/>
         <v>python AStar.py EightPuzzleWithHeuristics h_hamming puzzle12a</v>
       </c>
     </row>
@@ -1216,7 +1224,7 @@
         <v>5</v>
       </c>
       <c r="H20" t="str">
-        <f xml:space="preserve"> "python "&amp;B20&amp;" "&amp;A20&amp;" "&amp;G20&amp;" "&amp;C20</f>
+        <f t="shared" si="0"/>
         <v>python AStar.py EightPuzzleWithHeuristics h_euclidean puzzle12a</v>
       </c>
     </row>
@@ -1243,7 +1251,7 @@
         <v>6</v>
       </c>
       <c r="H21" t="str">
-        <f xml:space="preserve"> "python "&amp;B21&amp;" "&amp;A21&amp;" "&amp;G21&amp;" "&amp;C21</f>
+        <f t="shared" si="0"/>
         <v>python AStar.py EightPuzzleWithHeuristics h_manhattan puzzle12a</v>
       </c>
     </row>
@@ -1270,7 +1278,7 @@
         <v>7</v>
       </c>
       <c r="H22" t="str">
-        <f xml:space="preserve"> "python "&amp;B22&amp;" "&amp;A22&amp;" "&amp;G22&amp;" "&amp;C22</f>
+        <f t="shared" si="0"/>
         <v>python AStar.py EightPuzzleWithHeuristics h_custom puzzle12a</v>
       </c>
     </row>
@@ -1297,7 +1305,7 @@
         <v>4</v>
       </c>
       <c r="H23" t="str">
-        <f xml:space="preserve"> "python "&amp;B23&amp;" "&amp;A23&amp;" "&amp;G23&amp;" "&amp;C23</f>
+        <f t="shared" si="0"/>
         <v>python AStar.py EightPuzzleWithHeuristics h_hamming puzzle10a</v>
       </c>
     </row>
@@ -1324,7 +1332,7 @@
         <v>5</v>
       </c>
       <c r="H24" t="str">
-        <f xml:space="preserve"> "python "&amp;B24&amp;" "&amp;A24&amp;" "&amp;G24&amp;" "&amp;C24</f>
+        <f t="shared" si="0"/>
         <v>python AStar.py EightPuzzleWithHeuristics h_euclidean puzzle10a</v>
       </c>
     </row>
@@ -1351,7 +1359,7 @@
         <v>6</v>
       </c>
       <c r="H25" t="str">
-        <f xml:space="preserve"> "python "&amp;B25&amp;" "&amp;A25&amp;" "&amp;G25&amp;" "&amp;C25</f>
+        <f t="shared" si="0"/>
         <v>python AStar.py EightPuzzleWithHeuristics h_manhattan puzzle10a</v>
       </c>
     </row>
@@ -1378,7 +1386,7 @@
         <v>7</v>
       </c>
       <c r="H26" t="str">
-        <f xml:space="preserve"> "python "&amp;B26&amp;" "&amp;A26&amp;" "&amp;G26&amp;" "&amp;C26</f>
+        <f t="shared" si="0"/>
         <v>python AStar.py EightPuzzleWithHeuristics h_custom puzzle10a</v>
       </c>
     </row>
@@ -1405,7 +1413,7 @@
         <v>4</v>
       </c>
       <c r="H27" t="str">
-        <f xml:space="preserve"> "python "&amp;B27&amp;" "&amp;A27&amp;" "&amp;G27&amp;" "&amp;C27</f>
+        <f t="shared" si="0"/>
         <v>python AStar.py EightPuzzleWithHeuristics h_hamming puzzle14a</v>
       </c>
     </row>
@@ -1432,7 +1440,7 @@
         <v>5</v>
       </c>
       <c r="H28" t="str">
-        <f xml:space="preserve"> "python "&amp;B28&amp;" "&amp;A28&amp;" "&amp;G28&amp;" "&amp;C28</f>
+        <f t="shared" si="0"/>
         <v>python AStar.py EightPuzzleWithHeuristics h_euclidean puzzle14a</v>
       </c>
     </row>
@@ -1459,7 +1467,7 @@
         <v>6</v>
       </c>
       <c r="H29" t="str">
-        <f xml:space="preserve"> "python "&amp;B29&amp;" "&amp;A29&amp;" "&amp;G29&amp;" "&amp;C29</f>
+        <f t="shared" si="0"/>
         <v>python AStar.py EightPuzzleWithHeuristics h_manhattan puzzle14a</v>
       </c>
     </row>
@@ -1486,7 +1494,7 @@
         <v>7</v>
       </c>
       <c r="H30" t="str">
-        <f xml:space="preserve"> "python "&amp;B30&amp;" "&amp;A30&amp;" "&amp;G30&amp;" "&amp;C30</f>
+        <f t="shared" si="0"/>
         <v>python AStar.py EightPuzzleWithHeuristics h_custom puzzle14a</v>
       </c>
     </row>
@@ -1513,7 +1521,7 @@
         <v>4</v>
       </c>
       <c r="H31" t="str">
-        <f xml:space="preserve"> "python "&amp;B31&amp;" "&amp;A31&amp;" "&amp;G31&amp;" "&amp;C31</f>
+        <f t="shared" si="0"/>
         <v>python AStar.py EightPuzzleWithHeuristics h_hamming puzzle16a</v>
       </c>
     </row>
@@ -1540,7 +1548,7 @@
         <v>5</v>
       </c>
       <c r="H32" t="str">
-        <f xml:space="preserve"> "python "&amp;B32&amp;" "&amp;A32&amp;" "&amp;G32&amp;" "&amp;C32</f>
+        <f t="shared" si="0"/>
         <v>python AStar.py EightPuzzleWithHeuristics h_euclidean puzzle16a</v>
       </c>
     </row>
@@ -1567,7 +1575,7 @@
         <v>6</v>
       </c>
       <c r="H33" t="str">
-        <f xml:space="preserve"> "python "&amp;B33&amp;" "&amp;A33&amp;" "&amp;G33&amp;" "&amp;C33</f>
+        <f t="shared" si="0"/>
         <v>python AStar.py EightPuzzleWithHeuristics h_manhattan puzzle16a</v>
       </c>
     </row>
@@ -1594,7 +1602,7 @@
         <v>7</v>
       </c>
       <c r="H34" t="str">
-        <f xml:space="preserve"> "python "&amp;B34&amp;" "&amp;A34&amp;" "&amp;G34&amp;" "&amp;C34</f>
+        <f t="shared" si="0"/>
         <v>python AStar.py EightPuzzleWithHeuristics h_custom puzzle16a</v>
       </c>
     </row>
@@ -1618,7 +1626,7 @@
         <v>2</v>
       </c>
       <c r="H35" t="str">
-        <f xml:space="preserve"> "python "&amp;B35&amp;" "&amp;A35&amp;" "&amp;G35&amp;" "&amp;C35</f>
+        <f t="shared" si="0"/>
         <v>python ItrBFS.py EightPuzzleWithHeuristics  puzzle1a</v>
       </c>
     </row>
@@ -1642,7 +1650,7 @@
         <v>9</v>
       </c>
       <c r="H36" t="str">
-        <f xml:space="preserve"> "python "&amp;B36&amp;" "&amp;A36&amp;" "&amp;G36&amp;" "&amp;C36</f>
+        <f t="shared" si="0"/>
         <v>python ItrBFS.py EightPuzzleWithHeuristics  puzzle2a</v>
       </c>
     </row>
@@ -1666,7 +1674,7 @@
         <v>161</v>
       </c>
       <c r="H37" t="str">
-        <f xml:space="preserve"> "python "&amp;B37&amp;" "&amp;A37&amp;" "&amp;G37&amp;" "&amp;C37</f>
+        <f t="shared" si="0"/>
         <v>python ItrBFS.py EightPuzzleWithHeuristics  puzzle4a</v>
       </c>
     </row>
@@ -1690,7 +1698,7 @@
         <v>3375</v>
       </c>
       <c r="H38" t="str">
-        <f xml:space="preserve"> "python "&amp;B38&amp;" "&amp;A38&amp;" "&amp;G38&amp;" "&amp;C38</f>
+        <f t="shared" si="0"/>
         <v>python ItrBFS.py EightPuzzleWithHeuristics  puzzle10a</v>
       </c>
     </row>
@@ -1714,7 +1722,7 @@
         <v>946</v>
       </c>
       <c r="H39" t="str">
-        <f xml:space="preserve"> "python "&amp;B39&amp;" "&amp;A39&amp;" "&amp;G39&amp;" "&amp;C39</f>
+        <f t="shared" si="0"/>
         <v>python ItrBFS.py EightPuzzleWithHeuristics  puzzle12a</v>
       </c>
     </row>
@@ -1732,7 +1740,7 @@
         <v>25</v>
       </c>
       <c r="H40" t="str">
-        <f xml:space="preserve"> "python "&amp;B40&amp;" "&amp;A40&amp;" "&amp;G40&amp;" "&amp;C40</f>
+        <f t="shared" si="0"/>
         <v>python ItrBFS.py EightPuzzleWithHeuristics  puzzle14a</v>
       </c>
     </row>
@@ -1750,7 +1758,7 @@
         <v>26</v>
       </c>
       <c r="H41" t="str">
-        <f xml:space="preserve"> "python "&amp;B41&amp;" "&amp;A41&amp;" "&amp;G41&amp;" "&amp;C41</f>
+        <f t="shared" si="0"/>
         <v>python ItrBFS.py EightPuzzleWithHeuristics  puzzle16a</v>
       </c>
     </row>
@@ -1768,7 +1776,7 @@
         <v>22</v>
       </c>
       <c r="H42" t="str">
-        <f xml:space="preserve"> "python "&amp;B42&amp;" "&amp;A42&amp;" "&amp;G42&amp;" "&amp;C42</f>
+        <f t="shared" si="0"/>
         <v>python ItrBFS.py BasicEightPuzzle  puzzle0</v>
       </c>
     </row>
@@ -1786,7 +1794,7 @@
         <v>27</v>
       </c>
       <c r="H43" t="str">
-        <f xml:space="preserve"> "python "&amp;B43&amp;" "&amp;A43&amp;" "&amp;G43&amp;" "&amp;C43</f>
+        <f t="shared" si="0"/>
         <v>python ItrBFS.py BasicEightPuzzle  puzzle1a</v>
       </c>
     </row>
@@ -1804,7 +1812,7 @@
         <v>28</v>
       </c>
       <c r="H44" t="str">
-        <f xml:space="preserve"> "python "&amp;B44&amp;" "&amp;A44&amp;" "&amp;G44&amp;" "&amp;C44</f>
+        <f t="shared" si="0"/>
         <v>python ItrBFS.py BasicEightPuzzle  puzzle2a</v>
       </c>
     </row>
@@ -1822,7 +1830,7 @@
         <v>29</v>
       </c>
       <c r="H45" t="str">
-        <f xml:space="preserve"> "python "&amp;B45&amp;" "&amp;A45&amp;" "&amp;G45&amp;" "&amp;C45</f>
+        <f t="shared" si="0"/>
         <v>python ItrBFS.py BasicEightPuzzle  puzzle4a</v>
       </c>
     </row>
@@ -1840,7 +1848,7 @@
         <v>23</v>
       </c>
       <c r="H46" t="str">
-        <f xml:space="preserve"> "python "&amp;B46&amp;" "&amp;A46&amp;" "&amp;G46&amp;" "&amp;C46</f>
+        <f t="shared" si="0"/>
         <v>python ItrBFS.py BasicEightPuzzle  puzzle10a</v>
       </c>
     </row>
@@ -1858,7 +1866,7 @@
         <v>24</v>
       </c>
       <c r="H47" t="str">
-        <f xml:space="preserve"> "python "&amp;B47&amp;" "&amp;A47&amp;" "&amp;G47&amp;" "&amp;C47</f>
+        <f t="shared" si="0"/>
         <v>python ItrBFS.py BasicEightPuzzle  puzzle12a</v>
       </c>
     </row>
@@ -1876,7 +1884,7 @@
         <v>25</v>
       </c>
       <c r="H48" t="str">
-        <f xml:space="preserve"> "python "&amp;B48&amp;" "&amp;A48&amp;" "&amp;G48&amp;" "&amp;C48</f>
+        <f t="shared" si="0"/>
         <v>python ItrBFS.py BasicEightPuzzle  puzzle14a</v>
       </c>
     </row>
@@ -1894,7 +1902,7 @@
         <v>26</v>
       </c>
       <c r="H49" t="str">
-        <f xml:space="preserve"> "python "&amp;B49&amp;" "&amp;A49&amp;" "&amp;G49&amp;" "&amp;C49</f>
+        <f t="shared" si="0"/>
         <v>python ItrBFS.py BasicEightPuzzle  puzzle16a</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Starting K In A Row Agent
</commit_message>
<xml_diff>
--- a/Assignment3/Comparison of Algorithms.xlsx
+++ b/Assignment3/Comparison of Algorithms.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16040" tabRatio="500"/>
+    <workbookView xWindow="13980" yWindow="2880" windowWidth="14820" windowHeight="13600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -187,9 +187,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="102">
+  <cellStyleXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -295,7 +299,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="102">
+  <cellStyles count="106">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -346,6 +350,8 @@
     <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="105" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -396,6 +402,8 @@
     <cellStyle name="Hyperlink" xfId="96" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="98" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="100" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="102" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="104" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -675,10 +683,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H49"/>
+  <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="D23" workbookViewId="0">
+      <selection activeCell="H34" sqref="H34:H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -692,7 +700,7 @@
     <col min="8" max="8" width="66.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -718,7 +726,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -738,14 +746,14 @@
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="H2" t="str">
-        <f t="shared" ref="H2:H49" si="0" xml:space="preserve"> "python "&amp;B2&amp;" "&amp;A2&amp;" "&amp;G2&amp;" "&amp;C2</f>
-        <v>python AStar.py EightPuzzleWithHeuristics h_hamming puzzle0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+        <f xml:space="preserve"> "python "&amp;B2&amp;" "&amp;A2&amp;" "&amp;G2&amp;" "&amp;C2</f>
+        <v>python AStar.py EightPuzzleWithHeuristics h_custom puzzle0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -753,53 +761,65 @@
         <v>19</v>
       </c>
       <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3">
+        <v>12</v>
+      </c>
+      <c r="F3">
+        <v>61</v>
+      </c>
+      <c r="G3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" t="str">
+        <f xml:space="preserve"> "python "&amp;B3&amp;" "&amp;A3&amp;" "&amp;G3&amp;" "&amp;C3</f>
+        <v>python AStar.py EightPuzzleWithHeuristics h_custom puzzle10a</v>
+      </c>
+      <c r="I3">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
+      <c r="J3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4">
+        <v>8</v>
+      </c>
+      <c r="F4">
         <v>22</v>
       </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H3" t="str">
-        <f t="shared" si="0"/>
-        <v>python AStar.py EightPuzzleWithHeuristics h_euclidean puzzle0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
       <c r="G4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H4" t="str">
-        <f t="shared" si="0"/>
-        <v>python AStar.py EightPuzzleWithHeuristics h_manhattan puzzle0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+        <f xml:space="preserve"> "python "&amp;B4&amp;" "&amp;A4&amp;" "&amp;G4&amp;" "&amp;C4</f>
+        <v>python AStar.py EightPuzzleWithHeuristics h_custom puzzle12a</v>
+      </c>
+      <c r="I4">
+        <v>8</v>
+      </c>
+      <c r="J4">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -807,26 +827,32 @@
         <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>194</v>
       </c>
       <c r="G5" t="s">
         <v>7</v>
       </c>
       <c r="H5" t="str">
-        <f t="shared" si="0"/>
-        <v>python AStar.py EightPuzzleWithHeuristics h_custom puzzle0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+        <f xml:space="preserve"> "python "&amp;B5&amp;" "&amp;A5&amp;" "&amp;G5&amp;" "&amp;C5</f>
+        <v>python AStar.py EightPuzzleWithHeuristics h_custom puzzle14a</v>
+      </c>
+      <c r="I5">
+        <v>14</v>
+      </c>
+      <c r="J5">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -834,26 +860,32 @@
         <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>285</v>
       </c>
       <c r="G6" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="H6" t="str">
-        <f t="shared" si="0"/>
-        <v>python AStar.py EightPuzzleWithHeuristics h_hamming puzzle1a</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+        <f xml:space="preserve"> "python "&amp;B6&amp;" "&amp;A6&amp;" "&amp;G6&amp;" "&amp;C6</f>
+        <v>python AStar.py EightPuzzleWithHeuristics h_custom puzzle16a</v>
+      </c>
+      <c r="I6">
+        <v>16</v>
+      </c>
+      <c r="J6">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -873,73 +905,73 @@
         <v>1</v>
       </c>
       <c r="G7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7" t="str">
+        <f xml:space="preserve"> "python "&amp;B7&amp;" "&amp;A7&amp;" "&amp;G7&amp;" "&amp;C7</f>
+        <v>python AStar.py EightPuzzleWithHeuristics h_custom puzzle1a</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" t="str">
+        <f xml:space="preserve"> "python "&amp;B8&amp;" "&amp;A8&amp;" "&amp;G8&amp;" "&amp;C8</f>
+        <v>python AStar.py EightPuzzleWithHeuristics h_custom puzzle2a</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9">
         <v>5</v>
       </c>
-      <c r="H7" t="str">
-        <f t="shared" si="0"/>
-        <v>python AStar.py EightPuzzleWithHeuristics h_euclidean puzzle1a</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8" t="s">
-        <v>6</v>
-      </c>
-      <c r="H8" t="str">
-        <f t="shared" si="0"/>
-        <v>python AStar.py EightPuzzleWithHeuristics h_manhattan puzzle1a</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
       <c r="F9">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G9" t="s">
         <v>7</v>
       </c>
       <c r="H9" t="str">
-        <f t="shared" si="0"/>
-        <v>python AStar.py EightPuzzleWithHeuristics h_custom puzzle1a</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+        <f xml:space="preserve"> "python "&amp;B9&amp;" "&amp;A9&amp;" "&amp;G9&amp;" "&amp;C9</f>
+        <v>python AStar.py EightPuzzleWithHeuristics h_custom puzzle4a</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C10" t="s">
         <v>10</v>
@@ -948,17 +980,20 @@
         <v>22</v>
       </c>
       <c r="E10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="G10" t="s">
+        <v>5</v>
       </c>
       <c r="H10" t="str">
-        <f t="shared" si="0"/>
-        <v>python ItrBFS.py EightPuzzleWithHeuristics  puzzle0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+        <f xml:space="preserve"> "python "&amp;B10&amp;" "&amp;A10&amp;" "&amp;G10&amp;" "&amp;C10</f>
+        <v>python AStar.py EightPuzzleWithHeuristics h_euclidean puzzle0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -966,26 +1001,26 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E11">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F11">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="G11" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H11" t="str">
-        <f t="shared" si="0"/>
-        <v>python AStar.py EightPuzzleWithHeuristics h_hamming puzzle2a</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+        <f xml:space="preserve"> "python "&amp;B11&amp;" "&amp;A11&amp;" "&amp;G11&amp;" "&amp;C11</f>
+        <v>python AStar.py EightPuzzleWithHeuristics h_euclidean puzzle10a</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -993,26 +1028,26 @@
         <v>19</v>
       </c>
       <c r="C12" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D12" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E12">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F12">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="G12" t="s">
         <v>5</v>
       </c>
       <c r="H12" t="str">
-        <f t="shared" si="0"/>
-        <v>python AStar.py EightPuzzleWithHeuristics h_euclidean puzzle2a</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+        <f xml:space="preserve"> "python "&amp;B12&amp;" "&amp;A12&amp;" "&amp;G12&amp;" "&amp;C12</f>
+        <v>python AStar.py EightPuzzleWithHeuristics h_euclidean puzzle12a</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -1020,104 +1055,104 @@
         <v>19</v>
       </c>
       <c r="C13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13">
+        <v>14</v>
+      </c>
+      <c r="F13">
+        <v>144</v>
+      </c>
+      <c r="G13" t="s">
+        <v>5</v>
+      </c>
+      <c r="H13" t="str">
+        <f xml:space="preserve"> "python "&amp;B13&amp;" "&amp;A13&amp;" "&amp;G13&amp;" "&amp;C13</f>
+        <v>python AStar.py EightPuzzleWithHeuristics h_euclidean puzzle14a</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14">
+        <v>16</v>
+      </c>
+      <c r="F14">
+        <v>778</v>
+      </c>
+      <c r="G14" t="s">
+        <v>5</v>
+      </c>
+      <c r="H14" t="str">
+        <f xml:space="preserve"> "python "&amp;B14&amp;" "&amp;A14&amp;" "&amp;G14&amp;" "&amp;C14</f>
+        <v>python AStar.py EightPuzzleWithHeuristics h_euclidean puzzle16a</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15" t="s">
+        <v>5</v>
+      </c>
+      <c r="H15" t="str">
+        <f xml:space="preserve"> "python "&amp;B15&amp;" "&amp;A15&amp;" "&amp;G15&amp;" "&amp;C15</f>
+        <v>python AStar.py EightPuzzleWithHeuristics h_euclidean puzzle1a</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" t="s">
         <v>12</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D16" t="s">
         <v>28</v>
       </c>
-      <c r="E13">
+      <c r="E16">
         <v>2</v>
       </c>
-      <c r="F13">
+      <c r="F16">
         <v>2</v>
-      </c>
-      <c r="G13" t="s">
-        <v>6</v>
-      </c>
-      <c r="H13" t="str">
-        <f t="shared" si="0"/>
-        <v>python AStar.py EightPuzzleWithHeuristics h_manhattan puzzle2a</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" t="s">
-        <v>28</v>
-      </c>
-      <c r="E14">
-        <v>2</v>
-      </c>
-      <c r="F14">
-        <v>2</v>
-      </c>
-      <c r="G14" t="s">
-        <v>7</v>
-      </c>
-      <c r="H14" t="str">
-        <f t="shared" si="0"/>
-        <v>python AStar.py EightPuzzleWithHeuristics h_custom puzzle2a</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>3</v>
-      </c>
-      <c r="B15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" t="s">
-        <v>29</v>
-      </c>
-      <c r="E15">
-        <v>5</v>
-      </c>
-      <c r="F15">
-        <v>5</v>
-      </c>
-      <c r="G15" t="s">
-        <v>4</v>
-      </c>
-      <c r="H15" t="str">
-        <f t="shared" si="0"/>
-        <v>python AStar.py EightPuzzleWithHeuristics h_hamming puzzle4a</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>3</v>
-      </c>
-      <c r="B16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" t="s">
-        <v>29</v>
-      </c>
-      <c r="E16">
-        <v>5</v>
-      </c>
-      <c r="F16">
-        <v>5</v>
       </c>
       <c r="G16" t="s">
         <v>5</v>
       </c>
       <c r="H16" t="str">
-        <f t="shared" si="0"/>
-        <v>python AStar.py EightPuzzleWithHeuristics h_euclidean puzzle4a</v>
+        <f xml:space="preserve"> "python "&amp;B16&amp;" "&amp;A16&amp;" "&amp;G16&amp;" "&amp;C16</f>
+        <v>python AStar.py EightPuzzleWithHeuristics h_euclidean puzzle2a</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
@@ -1140,11 +1175,11 @@
         <v>5</v>
       </c>
       <c r="G17" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H17" t="str">
-        <f t="shared" si="0"/>
-        <v>python AStar.py EightPuzzleWithHeuristics h_manhattan puzzle4a</v>
+        <f xml:space="preserve"> "python "&amp;B17&amp;" "&amp;A17&amp;" "&amp;G17&amp;" "&amp;C17</f>
+        <v>python AStar.py EightPuzzleWithHeuristics h_euclidean puzzle4a</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
@@ -1155,23 +1190,23 @@
         <v>19</v>
       </c>
       <c r="C18" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D18" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="E18">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F18">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="G18" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H18" t="str">
-        <f t="shared" si="0"/>
-        <v>python AStar.py EightPuzzleWithHeuristics h_custom puzzle4a</v>
+        <f xml:space="preserve"> "python "&amp;B18&amp;" "&amp;A18&amp;" "&amp;G18&amp;" "&amp;C18</f>
+        <v>python AStar.py EightPuzzleWithHeuristics h_hamming puzzle0</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
@@ -1182,23 +1217,23 @@
         <v>19</v>
       </c>
       <c r="C19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E19">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F19">
-        <v>21</v>
+        <v>80</v>
       </c>
       <c r="G19" t="s">
         <v>4</v>
       </c>
       <c r="H19" t="str">
-        <f t="shared" si="0"/>
-        <v>python AStar.py EightPuzzleWithHeuristics h_hamming puzzle12a</v>
+        <f xml:space="preserve"> "python "&amp;B19&amp;" "&amp;A19&amp;" "&amp;G19&amp;" "&amp;C19</f>
+        <v>python AStar.py EightPuzzleWithHeuristics h_hamming puzzle10a</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
@@ -1218,14 +1253,14 @@
         <v>8</v>
       </c>
       <c r="F20">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="G20" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H20" t="str">
-        <f t="shared" si="0"/>
-        <v>python AStar.py EightPuzzleWithHeuristics h_euclidean puzzle12a</v>
+        <f xml:space="preserve"> "python "&amp;B20&amp;" "&amp;A20&amp;" "&amp;G20&amp;" "&amp;C20</f>
+        <v>python AStar.py EightPuzzleWithHeuristics h_hamming puzzle12a</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
@@ -1236,23 +1271,23 @@
         <v>19</v>
       </c>
       <c r="C21" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D21" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E21">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F21">
-        <v>29</v>
+        <v>524</v>
       </c>
       <c r="G21" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H21" t="str">
-        <f t="shared" si="0"/>
-        <v>python AStar.py EightPuzzleWithHeuristics h_manhattan puzzle12a</v>
+        <f xml:space="preserve"> "python "&amp;B21&amp;" "&amp;A21&amp;" "&amp;G21&amp;" "&amp;C21</f>
+        <v>python AStar.py EightPuzzleWithHeuristics h_hamming puzzle14a</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
@@ -1263,23 +1298,23 @@
         <v>19</v>
       </c>
       <c r="C22" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D22" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E22">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="F22">
-        <v>22</v>
+        <v>1552</v>
       </c>
       <c r="G22" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H22" t="str">
-        <f t="shared" si="0"/>
-        <v>python AStar.py EightPuzzleWithHeuristics h_custom puzzle12a</v>
+        <f xml:space="preserve"> "python "&amp;B22&amp;" "&amp;A22&amp;" "&amp;G22&amp;" "&amp;C22</f>
+        <v>python AStar.py EightPuzzleWithHeuristics h_hamming puzzle16a</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
@@ -1290,23 +1325,23 @@
         <v>19</v>
       </c>
       <c r="C23" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D23" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="E23">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F23">
-        <v>80</v>
+        <v>1</v>
       </c>
       <c r="G23" t="s">
         <v>4</v>
       </c>
       <c r="H23" t="str">
-        <f t="shared" si="0"/>
-        <v>python AStar.py EightPuzzleWithHeuristics h_hamming puzzle10a</v>
+        <f xml:space="preserve"> "python "&amp;B23&amp;" "&amp;A23&amp;" "&amp;G23&amp;" "&amp;C23</f>
+        <v>python AStar.py EightPuzzleWithHeuristics h_hamming puzzle1a</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
@@ -1317,23 +1352,23 @@
         <v>19</v>
       </c>
       <c r="C24" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D24" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="E24">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F24">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="G24" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H24" t="str">
-        <f t="shared" si="0"/>
-        <v>python AStar.py EightPuzzleWithHeuristics h_euclidean puzzle10a</v>
+        <f xml:space="preserve"> "python "&amp;B24&amp;" "&amp;A24&amp;" "&amp;G24&amp;" "&amp;C24</f>
+        <v>python AStar.py EightPuzzleWithHeuristics h_hamming puzzle2a</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
@@ -1344,23 +1379,23 @@
         <v>19</v>
       </c>
       <c r="C25" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D25" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="E25">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F25">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="G25" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H25" t="str">
-        <f t="shared" si="0"/>
-        <v>python AStar.py EightPuzzleWithHeuristics h_manhattan puzzle10a</v>
+        <f xml:space="preserve"> "python "&amp;B25&amp;" "&amp;A25&amp;" "&amp;G25&amp;" "&amp;C25</f>
+        <v>python AStar.py EightPuzzleWithHeuristics h_hamming puzzle4a</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
@@ -1371,23 +1406,23 @@
         <v>19</v>
       </c>
       <c r="C26" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D26" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E26">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="F26">
-        <v>61</v>
+        <v>0</v>
       </c>
       <c r="G26" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H26" t="str">
-        <f t="shared" si="0"/>
-        <v>python AStar.py EightPuzzleWithHeuristics h_custom puzzle10a</v>
+        <f xml:space="preserve"> "python "&amp;B26&amp;" "&amp;A26&amp;" "&amp;G26&amp;" "&amp;C26</f>
+        <v>python AStar.py EightPuzzleWithHeuristics h_manhattan puzzle0</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
@@ -1398,23 +1433,23 @@
         <v>19</v>
       </c>
       <c r="C27" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D27" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E27">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F27">
-        <v>524</v>
+        <v>21</v>
       </c>
       <c r="G27" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H27" t="str">
-        <f t="shared" si="0"/>
-        <v>python AStar.py EightPuzzleWithHeuristics h_hamming puzzle14a</v>
+        <f xml:space="preserve"> "python "&amp;B27&amp;" "&amp;A27&amp;" "&amp;G27&amp;" "&amp;C27</f>
+        <v>python AStar.py EightPuzzleWithHeuristics h_manhattan puzzle10a</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
@@ -1425,23 +1460,23 @@
         <v>19</v>
       </c>
       <c r="C28" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E28">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="F28">
-        <v>144</v>
+        <v>29</v>
       </c>
       <c r="G28" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H28" t="str">
-        <f t="shared" si="0"/>
-        <v>python AStar.py EightPuzzleWithHeuristics h_euclidean puzzle14a</v>
+        <f xml:space="preserve"> "python "&amp;B28&amp;" "&amp;A28&amp;" "&amp;G28&amp;" "&amp;C28</f>
+        <v>python AStar.py EightPuzzleWithHeuristics h_manhattan puzzle12a</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
@@ -1467,7 +1502,7 @@
         <v>6</v>
       </c>
       <c r="H29" t="str">
-        <f t="shared" si="0"/>
+        <f xml:space="preserve"> "python "&amp;B29&amp;" "&amp;A29&amp;" "&amp;G29&amp;" "&amp;C29</f>
         <v>python AStar.py EightPuzzleWithHeuristics h_manhattan puzzle14a</v>
       </c>
     </row>
@@ -1479,23 +1514,23 @@
         <v>19</v>
       </c>
       <c r="C30" t="s">
+        <v>17</v>
+      </c>
+      <c r="D30" t="s">
+        <v>26</v>
+      </c>
+      <c r="E30">
         <v>16</v>
       </c>
-      <c r="D30" t="s">
-        <v>25</v>
-      </c>
-      <c r="E30">
-        <v>14</v>
-      </c>
       <c r="F30">
-        <v>194</v>
+        <v>421</v>
       </c>
       <c r="G30" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H30" t="str">
-        <f t="shared" si="0"/>
-        <v>python AStar.py EightPuzzleWithHeuristics h_custom puzzle14a</v>
+        <f xml:space="preserve"> "python "&amp;B30&amp;" "&amp;A30&amp;" "&amp;G30&amp;" "&amp;C30</f>
+        <v>python AStar.py EightPuzzleWithHeuristics h_manhattan puzzle16a</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
@@ -1506,23 +1541,23 @@
         <v>19</v>
       </c>
       <c r="C31" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D31" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E31">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="F31">
-        <v>1552</v>
+        <v>1</v>
       </c>
       <c r="G31" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H31" t="str">
-        <f t="shared" si="0"/>
-        <v>python AStar.py EightPuzzleWithHeuristics h_hamming puzzle16a</v>
+        <f xml:space="preserve"> "python "&amp;B31&amp;" "&amp;A31&amp;" "&amp;G31&amp;" "&amp;C31</f>
+        <v>python AStar.py EightPuzzleWithHeuristics h_manhattan puzzle1a</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
@@ -1533,23 +1568,23 @@
         <v>19</v>
       </c>
       <c r="C32" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D32" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E32">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="F32">
-        <v>778</v>
+        <v>2</v>
       </c>
       <c r="G32" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H32" t="str">
-        <f t="shared" si="0"/>
-        <v>python AStar.py EightPuzzleWithHeuristics h_euclidean puzzle16a</v>
+        <f xml:space="preserve"> "python "&amp;B32&amp;" "&amp;A32&amp;" "&amp;G32&amp;" "&amp;C32</f>
+        <v>python AStar.py EightPuzzleWithHeuristics h_manhattan puzzle2a</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
@@ -1560,211 +1595,172 @@
         <v>19</v>
       </c>
       <c r="C33" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D33" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E33">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="F33">
-        <v>421</v>
+        <v>5</v>
       </c>
       <c r="G33" t="s">
         <v>6</v>
       </c>
       <c r="H33" t="str">
-        <f t="shared" si="0"/>
-        <v>python AStar.py EightPuzzleWithHeuristics h_manhattan puzzle16a</v>
+        <f xml:space="preserve"> "python "&amp;B33&amp;" "&amp;A33&amp;" "&amp;G33&amp;" "&amp;C33</f>
+        <v>python AStar.py EightPuzzleWithHeuristics h_manhattan puzzle4a</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="B34" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C34" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D34" t="s">
-        <v>26</v>
-      </c>
-      <c r="E34">
-        <v>16</v>
-      </c>
-      <c r="F34">
-        <v>285</v>
-      </c>
-      <c r="G34" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="H34" t="str">
-        <f t="shared" si="0"/>
-        <v>python AStar.py EightPuzzleWithHeuristics h_custom puzzle16a</v>
+        <f xml:space="preserve"> "python "&amp;B34&amp;" "&amp;A34&amp;" "&amp;G34&amp;" "&amp;C34</f>
+        <v>python ItrBFS.py BasicEightPuzzle  puzzle0</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="B35" t="s">
         <v>20</v>
       </c>
       <c r="C35" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D35" t="s">
-        <v>27</v>
-      </c>
-      <c r="E35">
-        <v>1</v>
-      </c>
-      <c r="F35">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="H35" t="str">
-        <f t="shared" si="0"/>
-        <v>python ItrBFS.py EightPuzzleWithHeuristics  puzzle1a</v>
+        <f xml:space="preserve"> "python "&amp;B35&amp;" "&amp;A35&amp;" "&amp;G35&amp;" "&amp;C35</f>
+        <v>python ItrBFS.py BasicEightPuzzle  puzzle10a</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="B36" t="s">
         <v>20</v>
       </c>
       <c r="C36" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D36" t="s">
-        <v>28</v>
-      </c>
-      <c r="E36">
-        <v>2</v>
-      </c>
-      <c r="F36">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="H36" t="str">
-        <f t="shared" si="0"/>
-        <v>python ItrBFS.py EightPuzzleWithHeuristics  puzzle2a</v>
+        <f xml:space="preserve"> "python "&amp;B36&amp;" "&amp;A36&amp;" "&amp;G36&amp;" "&amp;C36</f>
+        <v>python ItrBFS.py BasicEightPuzzle  puzzle12a</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="B37" t="s">
         <v>20</v>
       </c>
       <c r="C37" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D37" t="s">
-        <v>29</v>
-      </c>
-      <c r="E37">
-        <v>5</v>
-      </c>
-      <c r="F37">
-        <v>161</v>
+        <v>25</v>
       </c>
       <c r="H37" t="str">
-        <f t="shared" si="0"/>
-        <v>python ItrBFS.py EightPuzzleWithHeuristics  puzzle4a</v>
+        <f xml:space="preserve"> "python "&amp;B37&amp;" "&amp;A37&amp;" "&amp;G37&amp;" "&amp;C37</f>
+        <v>python ItrBFS.py BasicEightPuzzle  puzzle14a</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="B38" t="s">
         <v>20</v>
       </c>
       <c r="C38" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D38" t="s">
-        <v>23</v>
-      </c>
-      <c r="E38">
-        <v>10</v>
-      </c>
-      <c r="F38">
-        <v>3375</v>
+        <v>26</v>
       </c>
       <c r="H38" t="str">
-        <f t="shared" si="0"/>
-        <v>python ItrBFS.py EightPuzzleWithHeuristics  puzzle10a</v>
+        <f xml:space="preserve"> "python "&amp;B38&amp;" "&amp;A38&amp;" "&amp;G38&amp;" "&amp;C38</f>
+        <v>python ItrBFS.py BasicEightPuzzle  puzzle16a</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="B39" t="s">
         <v>20</v>
       </c>
       <c r="C39" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D39" t="s">
-        <v>24</v>
-      </c>
-      <c r="E39">
-        <v>8</v>
-      </c>
-      <c r="F39">
-        <v>946</v>
+        <v>27</v>
       </c>
       <c r="H39" t="str">
-        <f t="shared" si="0"/>
-        <v>python ItrBFS.py EightPuzzleWithHeuristics  puzzle12a</v>
+        <f xml:space="preserve"> "python "&amp;B39&amp;" "&amp;A39&amp;" "&amp;G39&amp;" "&amp;C39</f>
+        <v>python ItrBFS.py BasicEightPuzzle  puzzle1a</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="B40" t="s">
         <v>20</v>
       </c>
       <c r="C40" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D40" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H40" t="str">
-        <f t="shared" si="0"/>
-        <v>python ItrBFS.py EightPuzzleWithHeuristics  puzzle14a</v>
+        <f xml:space="preserve"> "python "&amp;B40&amp;" "&amp;A40&amp;" "&amp;G40&amp;" "&amp;C40</f>
+        <v>python ItrBFS.py BasicEightPuzzle  puzzle2a</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="B41" t="s">
         <v>20</v>
       </c>
       <c r="C41" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D41" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="H41" t="str">
-        <f t="shared" si="0"/>
-        <v>python ItrBFS.py EightPuzzleWithHeuristics  puzzle16a</v>
+        <f xml:space="preserve"> "python "&amp;B41&amp;" "&amp;A41&amp;" "&amp;G41&amp;" "&amp;C41</f>
+        <v>python ItrBFS.py BasicEightPuzzle  puzzle4a</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="B42" t="s">
         <v>20</v>
@@ -1775,140 +1771,176 @@
       <c r="D42" t="s">
         <v>22</v>
       </c>
+      <c r="E42">
+        <v>1</v>
+      </c>
+      <c r="F42">
+        <v>2</v>
+      </c>
       <c r="H42" t="str">
-        <f t="shared" si="0"/>
-        <v>python ItrBFS.py BasicEightPuzzle  puzzle0</v>
+        <f xml:space="preserve"> "python "&amp;B42&amp;" "&amp;A42&amp;" "&amp;G42&amp;" "&amp;C42</f>
+        <v>python ItrBFS.py EightPuzzleWithHeuristics  puzzle0</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="B43" t="s">
         <v>20</v>
       </c>
       <c r="C43" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D43" t="s">
-        <v>27</v>
+        <v>23</v>
+      </c>
+      <c r="E43">
+        <v>10</v>
+      </c>
+      <c r="F43">
+        <v>3375</v>
       </c>
       <c r="H43" t="str">
-        <f t="shared" si="0"/>
-        <v>python ItrBFS.py BasicEightPuzzle  puzzle1a</v>
+        <f xml:space="preserve"> "python "&amp;B43&amp;" "&amp;A43&amp;" "&amp;G43&amp;" "&amp;C43</f>
+        <v>python ItrBFS.py EightPuzzleWithHeuristics  puzzle10a</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="B44" t="s">
         <v>20</v>
       </c>
       <c r="C44" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D44" t="s">
-        <v>28</v>
+        <v>24</v>
+      </c>
+      <c r="E44">
+        <v>8</v>
+      </c>
+      <c r="F44">
+        <v>946</v>
       </c>
       <c r="H44" t="str">
-        <f t="shared" si="0"/>
-        <v>python ItrBFS.py BasicEightPuzzle  puzzle2a</v>
+        <f xml:space="preserve"> "python "&amp;B44&amp;" "&amp;A44&amp;" "&amp;G44&amp;" "&amp;C44</f>
+        <v>python ItrBFS.py EightPuzzleWithHeuristics  puzzle12a</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="B45" t="s">
         <v>20</v>
       </c>
       <c r="C45" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D45" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H45" t="str">
-        <f t="shared" si="0"/>
-        <v>python ItrBFS.py BasicEightPuzzle  puzzle4a</v>
+        <f xml:space="preserve"> "python "&amp;B45&amp;" "&amp;A45&amp;" "&amp;G45&amp;" "&amp;C45</f>
+        <v>python ItrBFS.py EightPuzzleWithHeuristics  puzzle14a</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="B46" t="s">
         <v>20</v>
       </c>
       <c r="C46" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D46" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="H46" t="str">
-        <f t="shared" si="0"/>
-        <v>python ItrBFS.py BasicEightPuzzle  puzzle10a</v>
+        <f xml:space="preserve"> "python "&amp;B46&amp;" "&amp;A46&amp;" "&amp;G46&amp;" "&amp;C46</f>
+        <v>python ItrBFS.py EightPuzzleWithHeuristics  puzzle16a</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="B47" t="s">
         <v>20</v>
       </c>
       <c r="C47" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D47" t="s">
-        <v>24</v>
+        <v>27</v>
+      </c>
+      <c r="E47">
+        <v>1</v>
+      </c>
+      <c r="F47">
+        <v>2</v>
       </c>
       <c r="H47" t="str">
-        <f t="shared" si="0"/>
-        <v>python ItrBFS.py BasicEightPuzzle  puzzle12a</v>
+        <f xml:space="preserve"> "python "&amp;B47&amp;" "&amp;A47&amp;" "&amp;G47&amp;" "&amp;C47</f>
+        <v>python ItrBFS.py EightPuzzleWithHeuristics  puzzle1a</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="B48" t="s">
         <v>20</v>
       </c>
       <c r="C48" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D48" t="s">
-        <v>25</v>
+        <v>28</v>
+      </c>
+      <c r="E48">
+        <v>2</v>
+      </c>
+      <c r="F48">
+        <v>9</v>
       </c>
       <c r="H48" t="str">
-        <f t="shared" si="0"/>
-        <v>python ItrBFS.py BasicEightPuzzle  puzzle14a</v>
+        <f xml:space="preserve"> "python "&amp;B48&amp;" "&amp;A48&amp;" "&amp;G48&amp;" "&amp;C48</f>
+        <v>python ItrBFS.py EightPuzzleWithHeuristics  puzzle2a</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="B49" t="s">
         <v>20</v>
       </c>
       <c r="C49" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D49" t="s">
-        <v>26</v>
+        <v>29</v>
+      </c>
+      <c r="E49">
+        <v>5</v>
+      </c>
+      <c r="F49">
+        <v>161</v>
       </c>
       <c r="H49" t="str">
-        <f t="shared" si="0"/>
-        <v>python ItrBFS.py BasicEightPuzzle  puzzle16a</v>
+        <f xml:space="preserve"> "python "&amp;B49&amp;" "&amp;A49&amp;" "&amp;G49&amp;" "&amp;C49</f>
+        <v>python ItrBFS.py EightPuzzleWithHeuristics  puzzle4a</v>
       </c>
     </row>
   </sheetData>
   <sortState ref="A2:H49">
-    <sortCondition ref="E1"/>
+    <sortCondition ref="H11"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>